<commit_message>
Actualizo tablas con los ultimos cambios
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/documentacion/Configuracion ruteo estatico.xlsx
+++ b/ tp-distribuidos-grupo3/documentacion/Configuracion ruteo estatico.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="74">
   <si>
     <t>Red</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>10.19.3.133</t>
-  </si>
-  <si>
-    <t>R8</t>
   </si>
   <si>
     <t>R9</t>
@@ -1017,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,225 +1046,225 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="18">
+        <v>255255255252</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D5" s="34">
         <v>255255255224</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D6" s="34">
         <v>255255255192</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D7" s="34">
+        <v>255255255252</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C8" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="34">
         <v>255255255128</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D9" s="34">
+        <v>255255255252</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D10" s="34">
         <v>255255255224</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D11" s="34">
         <v>255255255224</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C12" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="34">
         <v>255255255192</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="33" t="s">
         <v>5</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="9">
-        <v>255255255248</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="34">
+        <v>255255255248</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D15" s="37">
         <v>255255255240</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="18">
-        <v>255255255252</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D18" s="18">
+        <v>255255255252</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="D19" s="9">
         <v>255255255252</v>
@@ -1276,226 +1273,226 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="9">
+        <v>255255255252</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E21" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="9">
         <v>255255255224</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="9">
-        <v>255255255192</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="9">
+        <v>255255255192</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D24" s="9">
+        <v>255255255252</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D25" s="9">
         <v>255255255128</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="9">
-        <v>255255255252</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="9">
+        <v>255255255252</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D26" s="9">
-        <v>255255255224</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D27" s="9">
         <v>255255255224</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="9">
+        <v>255255255224</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D29" s="9">
         <v>255255255192</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="9">
-        <v>255255255248</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="9">
+        <v>255255255248</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D32" s="13">
         <v>255255255240</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="18">
-        <v>255255255252</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E35" s="10" t="s">
+      <c r="D35" s="18">
+        <v>255255255252</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="9">
         <v>255255255252</v>
@@ -1506,69 +1503,69 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D37" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D38" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D39" s="9">
-        <v>255255255252</v>
+        <v>255255255192</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="9">
-        <v>255255255128</v>
+        <v>255255255252</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D41" s="9">
-        <v>255255255252</v>
+        <v>255255255128</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>37</v>
@@ -1576,13 +1573,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D42" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>37</v>
@@ -1590,10 +1587,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D43" s="9">
         <v>255255255224</v>
@@ -1604,13 +1601,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>37</v>
@@ -1618,13 +1615,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="D45" s="9">
+        <v>255255255192</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>37</v>
@@ -1632,84 +1629,84 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="9">
-        <v>255255255248</v>
+        <v>30</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="9">
+        <v>255255255248</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C48" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D48" s="13">
         <v>255255255240</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E48" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="18">
-        <v>255255255252</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E51" s="10" t="s">
+      <c r="D51" s="18">
+        <v>255255255252</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" s="9">
         <v>255255255252</v>
@@ -1720,69 +1717,69 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D53" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D54" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D55" s="9">
-        <v>255255255252</v>
+        <v>255255255192</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56" s="9">
-        <v>255255255128</v>
+        <v>255255255252</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D57" s="9">
-        <v>255255255252</v>
+        <v>255255255128</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>37</v>
@@ -1790,13 +1787,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D58" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>37</v>
@@ -1804,10 +1801,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D59" s="9">
         <v>255255255224</v>
@@ -1818,13 +1815,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D60" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>37</v>
@@ -1832,13 +1829,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="D61" s="9">
+        <v>255255255192</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>37</v>
@@ -1846,86 +1843,86 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="9">
-        <v>255255255248</v>
+        <v>30</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="11" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="9">
+        <v>255255255248</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C64" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D64" s="13">
         <v>255255255240</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E64" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D67" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E67" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="15" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D67" s="19">
-        <v>255255255252</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D68" s="9">
+      <c r="D68" s="19">
         <v>255255255252</v>
       </c>
       <c r="E68" s="22" t="s">
@@ -1934,10 +1931,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D69" s="9">
         <v>255255255252</v>
@@ -1948,13 +1945,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D70" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>48</v>
@@ -1962,41 +1959,41 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D71" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D72" s="9">
-        <v>255255255252</v>
+        <v>255255255192</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D73" s="9">
-        <v>255255255128</v>
+        <v>255255255252</v>
       </c>
       <c r="E73" s="22" t="s">
         <v>48</v>
@@ -2004,13 +2001,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D74" s="9">
-        <v>255255255252</v>
+        <v>255255255128</v>
       </c>
       <c r="E74" s="22" t="s">
         <v>48</v>
@@ -2018,296 +2015,319 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D75" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D76" s="9">
         <v>255255255224</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D77" s="9">
-        <v>255255255192</v>
+        <v>255255255224</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="D78" s="9">
+        <v>255255255192</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D79" s="9">
-        <v>255255255248</v>
+        <v>30</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E79" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="11" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="9">
+        <v>255255255248</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C81" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D80" s="13">
+      <c r="D81" s="13">
         <v>255255255240</v>
       </c>
-      <c r="E80" s="23" t="s">
+      <c r="E81" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>51</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E82" s="20" t="s">
+      <c r="E83" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D84" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="21" t="s">
+      <c r="E84" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="7" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D84" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E84" s="22" t="s">
+      <c r="D85" s="9">
+        <v>255255255252</v>
+      </c>
+      <c r="E85" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="11" t="s">
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C86" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="24" t="s">
+      <c r="D86" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E85" s="23" t="s">
+      <c r="E86" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>53</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="11" t="s">
+    <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="12" t="s">
+      <c r="C89" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D88" s="26">
+      <c r="D89" s="26">
         <v>255255255192</v>
       </c>
-      <c r="E88" s="25" t="s">
+      <c r="E89" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="B91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E93" s="21" t="s">
+      <c r="B93" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D93" s="19">
+        <v>255255255252</v>
+      </c>
+      <c r="E93" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D94" s="19">
+      <c r="B94" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D94" s="9">
         <v>255255255252</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D95" s="9">
         <v>255255255252</v>
       </c>
       <c r="E95" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D96" s="9">
-        <v>255255255252</v>
+        <v>4</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E96" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="D97" s="9">
+        <v>255255255224</v>
       </c>
       <c r="E97" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D98" s="9">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E98" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D99" s="9">
-        <v>255255255252</v>
+        <v>255255255128</v>
       </c>
       <c r="E99" s="22" t="s">
         <v>57</v>
@@ -2315,264 +2335,264 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D100" s="9">
-        <v>255255255128</v>
+        <v>255255255252</v>
       </c>
       <c r="E100" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D101" s="9">
-        <v>255255255252</v>
+        <v>255255255224</v>
       </c>
       <c r="E101" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B102" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D102" s="9">
-        <v>255255255224</v>
+        <v>30</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E102" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B103" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D103" s="9">
+        <v>255255255248</v>
+      </c>
+      <c r="E103" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" s="13">
+        <v>255255255240</v>
+      </c>
+      <c r="E104" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>58</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C108" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D108" s="34">
+        <v>255255255252</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E109" s="42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" s="34">
+        <v>255255255224</v>
+      </c>
+      <c r="E110" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="34">
+        <v>255255255192</v>
+      </c>
+      <c r="E111" s="42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D112" s="34">
+        <v>255255255252</v>
+      </c>
+      <c r="E112" s="42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" s="34">
+        <v>255255255128</v>
+      </c>
+      <c r="E113" s="42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114" s="34">
+        <v>255255255224</v>
+      </c>
+      <c r="E114" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D115" s="34">
+        <v>255255255192</v>
+      </c>
+      <c r="E115" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C116" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="D116" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="7" t="s">
+      <c r="E116" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C117" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D117" s="34">
         <v>255255255248</v>
       </c>
-      <c r="E104" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="11" t="s">
+      <c r="E117" s="42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C118" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D105" s="13">
+      <c r="D118" s="37">
         <v>255255255240</v>
       </c>
-      <c r="E105" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>59</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E108" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D110" s="9">
-        <v>255255255224</v>
-      </c>
-      <c r="E110" s="22" t="s">
+      <c r="E118" s="43" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="9">
-        <v>255255255192</v>
-      </c>
-      <c r="E111" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D112" s="9">
-        <v>255255255252</v>
-      </c>
-      <c r="E112" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D113" s="9">
-        <v>255255255128</v>
-      </c>
-      <c r="E113" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D114" s="9">
-        <v>255255255224</v>
-      </c>
-      <c r="E114" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D115" s="9">
-        <v>255255255192</v>
-      </c>
-      <c r="E115" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E116" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D117" s="9">
-        <v>255255255248</v>
-      </c>
-      <c r="E117" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C118" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D118" s="13">
-        <v>255255255240</v>
-      </c>
-      <c r="E118" s="23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>0</v>
@@ -2598,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="E121" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,7 +2632,7 @@
         <v>255255255252</v>
       </c>
       <c r="E122" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2626,7 +2646,7 @@
         <v>255255255252</v>
       </c>
       <c r="E123" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -2640,7 +2660,7 @@
         <v>255255255252</v>
       </c>
       <c r="E124" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,7 +2674,7 @@
         <v>5</v>
       </c>
       <c r="E125" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2668,7 +2688,7 @@
         <v>255255255224</v>
       </c>
       <c r="E126" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,7 +2702,7 @@
         <v>255255255192</v>
       </c>
       <c r="E127" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,7 +2716,7 @@
         <v>255255255252</v>
       </c>
       <c r="E128" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2710,7 +2730,7 @@
         <v>255255255128</v>
       </c>
       <c r="E129" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -2724,7 +2744,7 @@
         <v>255255255252</v>
       </c>
       <c r="E130" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -2738,7 +2758,7 @@
         <v>255255255224</v>
       </c>
       <c r="E131" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -2752,7 +2772,7 @@
         <v>255255255192</v>
       </c>
       <c r="E132" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,7 +2786,7 @@
         <v>255255255248</v>
       </c>
       <c r="E133" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2780,13 +2800,13 @@
         <v>255255255240</v>
       </c>
       <c r="E134" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B136" s="27" t="s">
         <v>0</v>
@@ -2812,7 +2832,7 @@
         <v>5</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -2826,7 +2846,7 @@
         <v>255255255252</v>
       </c>
       <c r="E138" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -2840,7 +2860,7 @@
         <v>255255255252</v>
       </c>
       <c r="E139" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -2854,7 +2874,7 @@
         <v>255255255252</v>
       </c>
       <c r="E140" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -2868,7 +2888,7 @@
         <v>5</v>
       </c>
       <c r="E141" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -2882,7 +2902,7 @@
         <v>255255255224</v>
       </c>
       <c r="E142" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -2896,7 +2916,7 @@
         <v>255255255192</v>
       </c>
       <c r="E143" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,7 +2930,7 @@
         <v>255255255252</v>
       </c>
       <c r="E144" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -2924,7 +2944,7 @@
         <v>255255255128</v>
       </c>
       <c r="E145" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,7 +2958,7 @@
         <v>255255255252</v>
       </c>
       <c r="E146" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,7 +2972,7 @@
         <v>255255255224</v>
       </c>
       <c r="E147" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,7 +2986,7 @@
         <v>255255255224</v>
       </c>
       <c r="E148" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -2980,27 +3000,27 @@
         <v>255255255192</v>
       </c>
       <c r="E149" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B150" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C150" s="36" t="s">
         <v>69</v>
-      </c>
-      <c r="C150" s="36" t="s">
-        <v>70</v>
       </c>
       <c r="D150" s="37">
         <v>255255255248</v>
       </c>
       <c r="E150" s="43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="152" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B152" s="27" t="s">
         <v>0</v>
@@ -3026,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="E153" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3040,7 +3060,7 @@
         <v>255255255252</v>
       </c>
       <c r="E154" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3054,7 +3074,7 @@
         <v>255255255252</v>
       </c>
       <c r="E155" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3068,7 +3088,7 @@
         <v>255255255252</v>
       </c>
       <c r="E156" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3082,7 +3102,7 @@
         <v>5</v>
       </c>
       <c r="E157" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3096,7 +3116,7 @@
         <v>255255255224</v>
       </c>
       <c r="E158" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3110,7 +3130,7 @@
         <v>255255255192</v>
       </c>
       <c r="E159" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3124,7 +3144,7 @@
         <v>255255255252</v>
       </c>
       <c r="E160" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
@@ -3138,7 +3158,7 @@
         <v>255255255128</v>
       </c>
       <c r="E161" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -3152,7 +3172,7 @@
         <v>255255255252</v>
       </c>
       <c r="E162" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
@@ -3166,7 +3186,7 @@
         <v>255255255224</v>
       </c>
       <c r="E163" s="42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
@@ -3180,7 +3200,7 @@
         <v>255255255224</v>
       </c>
       <c r="E164" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
@@ -3194,35 +3214,21 @@
         <v>255255255192</v>
       </c>
       <c r="E165" s="42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C166" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D166" s="34">
-        <v>255255255248</v>
-      </c>
-      <c r="E166" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="167" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C167" s="36" t="s">
+      <c r="C166" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D167" s="37">
+      <c r="D166" s="37">
         <v>255255255240</v>
       </c>
-      <c r="E167" s="43" t="s">
-        <v>67</v>
+      <c r="E166" s="43" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>